<commit_message>
ya se ven los datos en front end
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\OneDrive\Desktop\Auction house api\Auction-house\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\OneDrive\Desktop\Auction house api\Auction-house\Auction-house-Profit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBC6199-73BA-4BBF-88A7-4132960BFC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02FA237-3FB6-499A-BE5B-1BF096672ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14115" yWindow="-12585" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="192">
   <si>
     <t>Nº</t>
   </si>
@@ -605,6 +605,18 @@
   </si>
   <si>
     <t>Profit</t>
+  </si>
+  <si>
+    <t>Bone-Melted Faceplate</t>
+  </si>
+  <si>
+    <t>glorious legplates</t>
+  </si>
+  <si>
+    <t>glorious legplates of the fireflash</t>
+  </si>
+  <si>
+    <t>glorious legplates of the quickblade</t>
   </si>
 </sst>
 </file>
@@ -726,7 +738,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -814,11 +826,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -938,6 +970,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -945,6 +983,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3246,22 +3287,22 @@
       <c r="H11" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I11" s="41" t="s">
+      <c r="I11" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="41" t="s">
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="43"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="45"/>
     </row>
     <row r="12" spans="8:36" x14ac:dyDescent="0.25">
       <c r="H12" s="16" t="s">
@@ -4560,10 +4601,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:M22"/>
+  <dimension ref="B2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4585,16 +4626,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
       <c r="K2" s="34" t="s">
         <v>3</v>
       </c>
@@ -5117,6 +5158,62 @@
       <c r="G22" s="40"/>
       <c r="H22" s="40"/>
       <c r="I22" s="40"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="42">
+        <v>20</v>
+      </c>
+      <c r="E23" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="42">
+        <v>1</v>
+      </c>
+      <c r="E24" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" s="42">
+        <v>1</v>
+      </c>
+      <c r="E25" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="42">
+        <v>1</v>
+      </c>
+      <c r="E26" s="47">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>